<commit_message>
Fix cross-year date range handling in HR attendance module - Updated calculate_date_month to extract and handle years from date range string - Fixed detect_holidays_staffs to correctly handle dates spanning multiple years (e.g., Dec 2025 to Jan 2026) - Updated merge_files_staffs to properly infer year for cross-year ranges - Modified hr_attendance.py to auto-detect years from date columns
</commit_message>
<xml_diff>
--- a/data/template_exempted.xlsx
+++ b/data/template_exempted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="20730" windowHeight="9030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="20730" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="late" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="376">
   <si>
     <t>Emp ID</t>
   </si>
@@ -1131,22 +1131,19 @@
     <t>Himangshu Patowary</t>
   </si>
   <si>
-    <t>CL</t>
-  </si>
-  <si>
-    <t>SSA Panbazar</t>
-  </si>
-  <si>
-    <t>CA Office</t>
-  </si>
-  <si>
-    <t>Bus Late</t>
-  </si>
-  <si>
     <t>Geetanjali Gogoi</t>
   </si>
   <si>
     <t>GCU030180</t>
+  </si>
+  <si>
+    <t>Bhagyashree Mahanta</t>
+  </si>
+  <si>
+    <t>Fariza Saidin</t>
+  </si>
+  <si>
+    <t>Bus late</t>
   </si>
 </sst>
 </file>
@@ -1182,9 +1179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1484,18 +1484,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P144"/>
+  <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
@@ -1609,7 +1609,12 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D6" t="s">
+        <v>375</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
@@ -1629,18 +1634,8 @@
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1">
-        <v>45922</v>
-      </c>
-      <c r="D8" t="s">
-        <v>374</v>
-      </c>
-      <c r="E8" s="1">
-        <v>45924</v>
-      </c>
-      <c r="F8" t="s">
-        <v>374</v>
-      </c>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
@@ -1669,7 +1664,12 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D11" t="s">
+        <v>375</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:16">
@@ -1750,18 +1750,8 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D20" t="s">
-        <v>374</v>
-      </c>
-      <c r="E20" s="1">
-        <v>45925</v>
-      </c>
-      <c r="F20" t="s">
-        <v>374</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="G20" s="1"/>
       <c r="I20" s="1"/>
       <c r="K20" s="1"/>
@@ -1805,18 +1795,8 @@
       <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="1">
-        <v>45922</v>
-      </c>
-      <c r="D25" t="s">
-        <v>374</v>
-      </c>
-      <c r="E25" s="1">
-        <v>45924</v>
-      </c>
-      <c r="F25" t="s">
-        <v>374</v>
-      </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
@@ -1886,7 +1866,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1894,7 +1874,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -1902,7 +1882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>173</v>
       </c>
@@ -1910,7 +1890,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -1918,7 +1898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1927,7 +1907,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>175</v>
       </c>
@@ -1936,7 +1916,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>176</v>
       </c>
@@ -1944,7 +1924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>177</v>
       </c>
@@ -1952,27 +1932,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>178</v>
       </c>
       <c r="B41" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="1">
-        <v>45922</v>
-      </c>
-      <c r="D41" t="s">
-        <v>374</v>
-      </c>
-      <c r="E41" s="1">
-        <v>45924</v>
-      </c>
-      <c r="F41" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="C41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1980,7 +1950,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -1988,7 +1958,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -1996,7 +1966,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>181</v>
       </c>
@@ -2004,7 +1974,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>182</v>
       </c>
@@ -2012,7 +1982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>183</v>
       </c>
@@ -2020,7 +1990,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>184</v>
       </c>
@@ -2259,7 +2229,12 @@
       <c r="B76" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="1"/>
+      <c r="C76" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D76" t="s">
+        <v>375</v>
+      </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5">
@@ -2417,7 +2392,12 @@
       <c r="B95" t="s">
         <v>116</v>
       </c>
-      <c r="C95" s="1"/>
+      <c r="C95" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>375</v>
+      </c>
       <c r="E95" s="1"/>
       <c r="G95" s="1"/>
     </row>
@@ -2460,12 +2440,7 @@
       <c r="B100" t="s">
         <v>121</v>
       </c>
-      <c r="C100" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D100" t="s">
-        <v>374</v>
-      </c>
+      <c r="C100" s="1"/>
       <c r="E100" s="1"/>
       <c r="G100" s="1"/>
       <c r="I100" s="1"/>
@@ -2496,18 +2471,8 @@
       <c r="B103" t="s">
         <v>124</v>
       </c>
-      <c r="C103" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D103" t="s">
-        <v>374</v>
-      </c>
-      <c r="E103" s="1">
-        <v>45925</v>
-      </c>
-      <c r="F103" t="s">
-        <v>374</v>
-      </c>
+      <c r="C103" s="1"/>
+      <c r="E103" s="1"/>
       <c r="G103" s="1"/>
       <c r="I103" s="1"/>
       <c r="K103" s="1"/>
@@ -2609,7 +2574,12 @@
       <c r="B115" t="s">
         <v>138</v>
       </c>
-      <c r="C115" s="1"/>
+      <c r="C115" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D115" t="s">
+        <v>375</v>
+      </c>
       <c r="E115" s="1"/>
       <c r="G115" s="1"/>
     </row>
@@ -2712,7 +2682,12 @@
       <c r="B126" t="s">
         <v>269</v>
       </c>
-      <c r="C126" s="1"/>
+      <c r="C126" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D126" t="s">
+        <v>375</v>
+      </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:15">
@@ -2761,7 +2736,12 @@
       <c r="B131" t="s">
         <v>274</v>
       </c>
-      <c r="C131" s="1"/>
+      <c r="C131" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D131" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="132" spans="1:15">
       <c r="A132" t="s">
@@ -2779,18 +2759,8 @@
       <c r="B133" t="s">
         <v>291</v>
       </c>
-      <c r="C133" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D133" t="s">
-        <v>374</v>
-      </c>
-      <c r="E133" s="1">
-        <v>45925</v>
-      </c>
-      <c r="F133" t="s">
-        <v>374</v>
-      </c>
+      <c r="C133" s="1"/>
+      <c r="E133" s="1"/>
       <c r="G133" s="1"/>
       <c r="I133" s="1"/>
       <c r="K133" s="1"/>
@@ -2832,12 +2802,7 @@
       <c r="B136" t="s">
         <v>342</v>
       </c>
-      <c r="C136" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D136" t="s">
-        <v>374</v>
-      </c>
+      <c r="C136" s="1"/>
       <c r="E136" s="1"/>
       <c r="G136" s="1"/>
       <c r="I136" s="1"/>
@@ -2852,7 +2817,12 @@
       <c r="B137" t="s">
         <v>344</v>
       </c>
-      <c r="C137" s="1"/>
+      <c r="C137" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D137" t="s">
+        <v>375</v>
+      </c>
       <c r="E137" s="1"/>
       <c r="G137" s="1"/>
     </row>
@@ -2863,7 +2833,12 @@
       <c r="B138" t="s">
         <v>345</v>
       </c>
-      <c r="C138" s="1"/>
+      <c r="C138" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D138" t="s">
+        <v>375</v>
+      </c>
       <c r="E138" s="1"/>
       <c r="G138" s="1"/>
     </row>
@@ -2874,7 +2849,12 @@
       <c r="B139" t="s">
         <v>346</v>
       </c>
-      <c r="C139" s="1"/>
+      <c r="C139" s="1">
+        <v>45989</v>
+      </c>
+      <c r="D139" t="s">
+        <v>375</v>
+      </c>
       <c r="E139" s="1"/>
       <c r="G139" s="1"/>
     </row>
@@ -2915,38 +2895,31 @@
       <c r="B143" t="s">
         <v>361</v>
       </c>
-      <c r="C143" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D143" t="s">
-        <v>374</v>
-      </c>
-      <c r="E143" s="1">
-        <v>45925</v>
-      </c>
-      <c r="F143" t="s">
-        <v>374</v>
-      </c>
+      <c r="C143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="G143" s="1"/>
     </row>
     <row r="144" spans="1:15">
       <c r="A144" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B144" t="s">
-        <v>375</v>
-      </c>
-      <c r="C144" s="1">
-        <v>45922</v>
-      </c>
-      <c r="D144" t="s">
+        <v>371</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="E144" s="1"/>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="B145" t="s">
+        <v>373</v>
+      </c>
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="2:3">
+      <c r="B146" t="s">
         <v>374</v>
       </c>
-      <c r="E144" s="1">
-        <v>45924</v>
-      </c>
-      <c r="F144" t="s">
-        <v>374</v>
-      </c>
+      <c r="C146" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2958,8 +2931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="H131" sqref="H131"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3665,7 +3638,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>216</v>
       </c>
@@ -3673,7 +3646,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>217</v>
       </c>
@@ -3681,7 +3654,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>218</v>
       </c>
@@ -3689,7 +3662,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>219</v>
       </c>
@@ -3697,7 +3670,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>220</v>
       </c>
@@ -3705,7 +3678,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>221</v>
       </c>
@@ -3713,7 +3686,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>222</v>
       </c>
@@ -3721,15 +3694,17 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>223</v>
       </c>
       <c r="B88" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88" s="1"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>224</v>
       </c>
@@ -3737,7 +3712,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>225</v>
       </c>
@@ -3745,7 +3720,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>226</v>
       </c>
@@ -3753,7 +3728,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>227</v>
       </c>
@@ -3761,7 +3736,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>228</v>
       </c>
@@ -3769,7 +3744,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>229</v>
       </c>
@@ -3777,7 +3752,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>230</v>
       </c>
@@ -3785,7 +3760,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>231</v>
       </c>
@@ -3921,7 +3896,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
         <v>249</v>
       </c>
@@ -3929,7 +3904,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
         <v>250</v>
       </c>
@@ -3937,7 +3912,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
         <v>251</v>
       </c>
@@ -3945,7 +3920,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>252</v>
       </c>
@@ -3953,7 +3928,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>253</v>
       </c>
@@ -3961,7 +3936,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>254</v>
       </c>
@@ -3969,7 +3944,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>255</v>
       </c>
@@ -3977,7 +3952,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>256</v>
       </c>
@@ -3986,7 +3961,7 @@
       </c>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -3994,7 +3969,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>258</v>
       </c>
@@ -4002,7 +3977,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:7">
       <c r="A123" t="s">
         <v>259</v>
       </c>
@@ -4010,7 +3985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:7">
       <c r="A124" t="s">
         <v>260</v>
       </c>
@@ -4019,33 +3994,18 @@
       </c>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:7">
       <c r="A125" t="s">
         <v>279</v>
       </c>
       <c r="B125" t="s">
         <v>270</v>
       </c>
-      <c r="C125" s="1">
-        <v>45924</v>
-      </c>
-      <c r="D125" t="s">
-        <v>372</v>
-      </c>
-      <c r="E125" s="1">
-        <v>45925</v>
-      </c>
-      <c r="F125" t="s">
-        <v>372</v>
-      </c>
-      <c r="G125" s="1">
-        <v>45946</v>
-      </c>
-      <c r="H125" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="C125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126" t="s">
         <v>289</v>
       </c>
@@ -4054,7 +4014,7 @@
       </c>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:7">
       <c r="A127" t="s">
         <v>313</v>
       </c>
@@ -4063,7 +4023,7 @@
       </c>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:7">
       <c r="A128" t="s">
         <v>314</v>
       </c>
@@ -4262,8 +4222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6139,19 +6099,14 @@
       <c r="Q128" s="1"/>
       <c r="S128" s="1"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>332</v>
       </c>
       <c r="B129" t="s">
         <v>370</v>
       </c>
-      <c r="C129" s="1">
-        <v>45951</v>
-      </c>
-      <c r="D129" t="s">
-        <v>371</v>
-      </c>
+      <c r="C129" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>